<commit_message>
added standard error of the mean handling
</commit_message>
<xml_diff>
--- a/bootstrapit_results/bootstrapit_results_mean.xlsx
+++ b/bootstrapit_results/bootstrapit_results_mean.xlsx
@@ -399,7 +399,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>25.5877375</v>
+        <v>25.5938725</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -407,7 +407,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>26.924772</v>
+        <v>26.927938</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -415,7 +415,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>28.16094</v>
+        <v>28.15803833333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added errorbars capability to barchart
- errobar capability added
- removed barchart labels to an additional method
</commit_message>
<xml_diff>
--- a/bootstrapit_results/bootstrapit_results_mean.xlsx
+++ b/bootstrapit_results/bootstrapit_results_mean.xlsx
@@ -399,7 +399,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>25.5938725</v>
+        <v>25.58766625</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -407,7 +407,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>26.927938</v>
+        <v>26.920468</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -415,7 +415,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>28.15803833333334</v>
+        <v>28.16413500000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
barchart method returns its plot object
</commit_message>
<xml_diff>
--- a/bootstrapit_results/bootstrapit_results_mean.xlsx
+++ b/bootstrapit_results/bootstrapit_results_mean.xlsx
@@ -399,7 +399,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>25.58766625</v>
+        <v>25.5735975</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -407,7 +407,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>26.920468</v>
+        <v>26.92953</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -415,7 +415,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>28.16413500000001</v>
+        <v>28.17075166666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added and tested bootstrap median
</commit_message>
<xml_diff>
--- a/bootstrapit_results/bootstrapit_results_mean.xlsx
+++ b/bootstrapit_results/bootstrapit_results_mean.xlsx
@@ -399,7 +399,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>25.58807125</v>
+        <v>25.592455</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -407,7 +407,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>26.916714</v>
+        <v>26.924286</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -415,7 +415,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>28.17042833333333</v>
+        <v>28.16764333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
basic confidence interval plot working
</commit_message>
<xml_diff>
--- a/bootstrapit_results/bootstrapit_results_mean.xlsx
+++ b/bootstrapit_results/bootstrapit_results_mean.xlsx
@@ -14,18 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>mean</t>
   </si>
   <si>
-    <t>Brown</t>
+    <t>Wafer 1</t>
   </si>
   <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Blue</t>
+    <t>Wafer 2</t>
   </si>
 </sst>
 </file>
@@ -383,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -399,7 +396,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>25.592455</v>
+        <v>0.4832801460336079</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -407,15 +404,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>26.924286</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>28.16764333333333</v>
+        <v>0.4822122652746012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>